<commit_message>
add clustering and anomaly detection
</commit_message>
<xml_diff>
--- a/Orange/Ensemble-Bagging-Predictions-2.xlsx
+++ b/Orange/Ensemble-Bagging-Predictions-2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/js/Dropbox/Repos/MLCourse/Untracked/Homework/HW7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/js/Dropbox/Repos/MLCourse/Orange/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="520" yWindow="960" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F635"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A616" workbookViewId="0">
+      <selection activeCell="D639" sqref="D639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14331,7 +14338,7 @@
       </c>
     </row>
     <row r="635" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F635">
+      <c r="F635" s="1">
         <f>COUNTIF(F2:F634, 1)/COUNT(F2:F634)</f>
         <v>0.5781990521327014</v>
       </c>

</xml_diff>